<commit_message>
Update power progression notes
</commit_message>
<xml_diff>
--- a/PowerProgression.xlsx
+++ b/PowerProgression.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bunch of uncommitted changes
</commit_message>
<xml_diff>
--- a/PowerProgression.xlsx
+++ b/PowerProgression.xlsx
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
     <col min="4" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="10.28515625" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" customWidth="1"/>
     <col min="18" max="18" width="21" customWidth="1"/>
     <col min="19" max="19" width="17.42578125" customWidth="1"/>
     <col min="20" max="21" width="14.28515625" customWidth="1"/>
@@ -793,6 +793,8 @@
       <c r="H14" t="s">
         <v>23</v>
       </c>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
@@ -810,6 +812,8 @@
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D16">
@@ -848,11 +852,23 @@
       <c r="P16">
         <v>300</v>
       </c>
-    </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>22</v>
       </c>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="15:19" x14ac:dyDescent="0.25">
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F16:O16">
@@ -868,5 +884,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>